<commit_message>
reorganize data from part 1
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6948D5-E8AC-5B4E-BCD3-EE606C2398CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D33679-4F58-EF41-9679-3AB09BB03980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="520" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Variable Name</t>
   </si>
@@ -44,18 +44,9 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Sex</t>
-  </si>
-  <si>
     <t>Number of people in household</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Male/Female/O/NA</t>
   </si>
   <si>
@@ -69,6 +60,27 @@
   </si>
   <si>
     <t>Age of individual</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>sixty</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Number_of_people_in_household</t>
   </si>
 </sst>
 </file>
@@ -417,218 +429,267 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>180</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>175</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>178</v>
+      </c>
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5" s="2">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>192</v>
+      </c>
+      <c r="B6">
+        <v>90</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>156</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>166</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9" s="2">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>155</v>
+      </c>
+      <c r="B10">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>145</v>
+      </c>
+      <c r="B11">
+        <v>7000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>165</v>
+      </c>
+      <c r="C12" s="2">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>133</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>166</v>
+      </c>
+      <c r="B14">
+        <v>55</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>77</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>75</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>59</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>75</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>154</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2">
         <v>72</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>62</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -646,6 +707,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -654,7 +716,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -680,7 +742,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -688,10 +750,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -705,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct the data and redo part 2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D33679-4F58-EF41-9679-3AB09BB03980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8657CBED-FA09-8B40-B586-E8BF905EEB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="520" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Number of people in household</t>
-  </si>
-  <si>
     <t>Male/Female/O/NA</t>
   </si>
   <si>
@@ -80,7 +77,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>Number_of_people_in_household</t>
+    <t>NPH</t>
+  </si>
+  <si>
+    <t>Number of people in household(NPH)</t>
   </si>
 </sst>
 </file>
@@ -429,26 +429,26 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -458,14 +458,14 @@
       <c r="B2">
         <v>80</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -475,31 +475,31 @@
       <c r="B3">
         <v>70</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
         <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
         <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -509,14 +509,14 @@
       <c r="B5">
         <v>76</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
         <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -526,14 +526,14 @@
       <c r="B6">
         <v>90</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -543,14 +543,14 @@
       <c r="B7">
         <v>55</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
         <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -560,14 +560,14 @@
       <c r="B8">
         <v>90</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
         <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -577,14 +577,14 @@
       <c r="B9">
         <v>110</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
         <v>75</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -594,14 +594,14 @@
       <c r="B10">
         <v>54</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -611,28 +611,28 @@
       <c r="B11">
         <v>7000</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
         <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>165</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
         <v>59</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -642,14 +642,14 @@
       <c r="B13">
         <v>45</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
         <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -659,14 +659,14 @@
       <c r="B14">
         <v>55</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
         <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -676,14 +676,14 @@
       <c r="B15">
         <v>50</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
         <v>72</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
@@ -742,7 +742,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -750,10 +750,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>